<commit_message>
docs : WBS 업데이트
</commit_message>
<xml_diff>
--- a/Docs/WBS/WBS_Team_BlueBird.xlsx
+++ b/Docs/WBS/WBS_Team_BlueBird.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zereo\Desktop\Project\ContentsIT_Capston_Design\Docs\WBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AC8557-0EB0-44C2-8A0F-DA575057064A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63B75348-017F-4201-9ABE-C0E7A3C4D85B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,7 +154,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="112">
   <si>
     <t>END</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -225,10 +225,6 @@
   </si>
   <si>
     <t>MILESTONE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>컨텐츠</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -600,6 +596,14 @@
   </si>
   <si>
     <t>시연동영상</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>텍스쳐</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>엔딩 일러스트</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1642,45 +1646,12 @@
     <xf numFmtId="0" fontId="13" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="13" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1756,6 +1727,36 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1802,6 +1803,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="13" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2176,83 +2180,83 @@
   <sheetData>
     <row r="1" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:21" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="108" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="108" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="109"/>
+      <c r="O2" s="109"/>
+      <c r="P2" s="109"/>
+      <c r="Q2" s="109"/>
+      <c r="R2" s="109"/>
+      <c r="S2" s="109"/>
+      <c r="T2" s="109"/>
+      <c r="U2" s="110"/>
+    </row>
+    <row r="3" spans="2:21" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B3" s="129" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="115" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="125" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="126"/>
+      <c r="F3" s="120" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="117" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="119"/>
+      <c r="N3" s="120" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="121"/>
+      <c r="P3" s="121"/>
+      <c r="Q3" s="122"/>
+      <c r="R3" s="117" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="119" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="120"/>
-      <c r="H2" s="120"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="120"/>
-      <c r="L2" s="120"/>
-      <c r="M2" s="120"/>
-      <c r="N2" s="120"/>
-      <c r="O2" s="120"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="120"/>
-      <c r="R2" s="120"/>
-      <c r="S2" s="120"/>
-      <c r="T2" s="120"/>
-      <c r="U2" s="121"/>
-    </row>
-    <row r="3" spans="2:21" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="140" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="126" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="136" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="137"/>
-      <c r="F3" s="131" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="132"/>
-      <c r="H3" s="132"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="128" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" s="129"/>
-      <c r="L3" s="129"/>
-      <c r="M3" s="130"/>
-      <c r="N3" s="131" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" s="132"/>
-      <c r="P3" s="132"/>
-      <c r="Q3" s="133"/>
-      <c r="R3" s="128" t="s">
-        <v>58</v>
-      </c>
-      <c r="S3" s="129"/>
-      <c r="T3" s="129"/>
-      <c r="U3" s="130"/>
+      <c r="S3" s="118"/>
+      <c r="T3" s="118"/>
+      <c r="U3" s="119"/>
     </row>
     <row r="4" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="141"/>
-      <c r="C4" s="127"/>
-      <c r="D4" s="138"/>
-      <c r="E4" s="139"/>
+      <c r="B4" s="130"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="128"/>
       <c r="F4" s="54" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" s="53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="54" t="s">
         <v>12</v>
@@ -2264,19 +2268,19 @@
         <v>14</v>
       </c>
       <c r="M4" s="53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N4" s="54" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O4" s="50" t="s">
         <v>13</v>
       </c>
       <c r="P4" s="50" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q4" s="53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R4" s="54" t="s">
         <v>12</v>
@@ -2292,16 +2296,16 @@
       </c>
     </row>
     <row r="5" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="122">
+      <c r="B5" s="111">
         <v>1</v>
       </c>
       <c r="C5" s="43">
         <v>44440</v>
       </c>
-      <c r="D5" s="142" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="143"/>
+      <c r="D5" s="131" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="132"/>
       <c r="F5" s="35"/>
       <c r="G5" s="51"/>
       <c r="H5" s="52"/>
@@ -2320,14 +2324,14 @@
       <c r="U5" s="34"/>
     </row>
     <row r="6" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="123"/>
-      <c r="C6" s="125" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="109" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="110"/>
+      <c r="B6" s="112"/>
+      <c r="C6" s="114" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="133" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="134"/>
       <c r="F6" s="38"/>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -2346,12 +2350,12 @@
       <c r="U6" s="34"/>
     </row>
     <row r="7" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="123"/>
-      <c r="C7" s="125"/>
-      <c r="D7" s="111" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="112"/>
+      <c r="B7" s="112"/>
+      <c r="C7" s="114"/>
+      <c r="D7" s="135" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="136"/>
       <c r="F7" s="33"/>
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
@@ -2370,12 +2374,12 @@
       <c r="U7" s="34"/>
     </row>
     <row r="8" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="123"/>
-      <c r="C8" s="125"/>
-      <c r="D8" s="113" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="114"/>
+      <c r="B8" s="112"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="137" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="138"/>
       <c r="F8" s="33"/>
       <c r="G8" s="32"/>
       <c r="H8" s="32"/>
@@ -2393,12 +2397,12 @@
       <c r="U8" s="34"/>
     </row>
     <row r="9" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="123"/>
-      <c r="C9" s="125"/>
-      <c r="D9" s="115" t="s">
+      <c r="B9" s="112"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="116"/>
+      <c r="E9" s="140"/>
       <c r="F9" s="35"/>
       <c r="G9" s="31"/>
       <c r="H9" s="32"/>
@@ -2417,12 +2421,12 @@
       <c r="U9" s="34"/>
     </row>
     <row r="10" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="123"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="117" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="118"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="114"/>
+      <c r="D10" s="141" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="142"/>
       <c r="F10" s="35"/>
       <c r="G10" s="31"/>
       <c r="H10" s="32"/>
@@ -2441,14 +2445,14 @@
       <c r="U10" s="34"/>
     </row>
     <row r="11" spans="2:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="124"/>
+      <c r="B11" s="113"/>
       <c r="C11" s="44">
         <v>44532</v>
       </c>
-      <c r="D11" s="134" t="s">
+      <c r="D11" s="123" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="135"/>
+      <c r="E11" s="124"/>
       <c r="F11" s="36"/>
       <c r="G11" s="37"/>
       <c r="H11" s="62"/>
@@ -2468,6 +2472,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
     <mergeCell ref="F2:U2"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B5:B11"/>
@@ -2484,8 +2490,6 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2505,8 +2509,8 @@
   </sheetPr>
   <dimension ref="B1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2523,54 +2527,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="148" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="148"/>
-      <c r="D1" s="148"/>
-      <c r="E1" s="148"/>
-      <c r="F1" s="148"/>
-      <c r="G1" s="148"/>
-      <c r="H1" s="148"/>
-      <c r="I1" s="148"/>
-      <c r="J1" s="148"/>
+      <c r="B1" s="147" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+      <c r="F1" s="147"/>
+      <c r="G1" s="147"/>
+      <c r="H1" s="147"/>
+      <c r="I1" s="147"/>
+      <c r="J1" s="147"/>
     </row>
     <row r="2" spans="2:12" ht="9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="147"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
-      <c r="H2" s="147"/>
-      <c r="I2" s="147"/>
-      <c r="J2" s="147"/>
+      <c r="B2" s="146"/>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="153" t="s">
-        <v>107</v>
-      </c>
-      <c r="C3" s="154"/>
-      <c r="D3" s="154"/>
+      <c r="B3" s="152" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="153"/>
+      <c r="D3" s="153"/>
       <c r="E3" s="10"/>
-      <c r="F3" s="151" t="s">
+      <c r="F3" s="150" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="151"/>
-      <c r="H3" s="151"/>
-      <c r="I3" s="151"/>
-      <c r="J3" s="151"/>
+      <c r="G3" s="150"/>
+      <c r="H3" s="150"/>
+      <c r="I3" s="150"/>
+      <c r="J3" s="150"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="154"/>
-      <c r="C4" s="154"/>
-      <c r="D4" s="154"/>
+      <c r="B4" s="153"/>
+      <c r="C4" s="153"/>
+      <c r="D4" s="153"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="152" t="s">
+      <c r="F4" s="151" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="152"/>
-      <c r="H4" s="152"/>
+      <c r="G4" s="151"/>
+      <c r="H4" s="151"/>
       <c r="I4" s="1" t="s">
         <v>11</v>
       </c>
@@ -2579,9 +2583,9 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="154"/>
-      <c r="C5" s="154"/>
-      <c r="D5" s="154"/>
+      <c r="B5" s="153"/>
+      <c r="C5" s="153"/>
+      <c r="D5" s="153"/>
       <c r="E5" s="10"/>
       <c r="F5" s="1" t="s">
         <v>3</v>
@@ -2594,20 +2598,20 @@
       </c>
       <c r="I5" s="3">
         <f>AVERAGE(I12,I19,I27,I45,I50,I55,I37)</f>
-        <v>41.870748299319736</v>
+        <v>43.367346938775505</v>
       </c>
       <c r="J5" s="2">
         <f>COUNTIF(J6:J55,"완료")</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L5" s="30"/>
     </row>
     <row r="6" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="144" t="s">
-        <v>32</v>
+      <c r="B6" s="143" t="s">
+        <v>31</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="11"/>
@@ -2627,9 +2631,9 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="149"/>
+      <c r="B7" s="148"/>
       <c r="C7" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="11"/>
@@ -2652,9 +2656,9 @@
       <c r="L7" s="30"/>
     </row>
     <row r="8" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="149"/>
+      <c r="B8" s="148"/>
       <c r="C8" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" s="39"/>
       <c r="E8" s="11"/>
@@ -2677,9 +2681,9 @@
       <c r="L8" s="30"/>
     </row>
     <row r="9" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="149"/>
+      <c r="B9" s="148"/>
       <c r="C9" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="12"/>
@@ -2699,9 +2703,9 @@
       </c>
     </row>
     <row r="10" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="149"/>
+      <c r="B10" s="148"/>
       <c r="C10" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D10" s="28"/>
       <c r="E10" s="12"/>
@@ -2713,17 +2717,17 @@
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J10" s="4" t="str">
         <f>IF(I10=100,"완료",IF(I10=0,"-","진행중"))</f>
-        <v>-</v>
+        <v>진행중</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="150"/>
+      <c r="B11" s="149"/>
       <c r="C11" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="12"/>
@@ -2752,7 +2756,7 @@
       <c r="H12" s="23"/>
       <c r="I12" s="17">
         <f>AVERAGE(I6:I11)</f>
-        <v>50</v>
+        <v>51.666666666666664</v>
       </c>
       <c r="J12" s="14">
         <f>COUNTIF(J6:J11,"완료")</f>
@@ -2760,11 +2764,11 @@
       </c>
     </row>
     <row r="13" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="144" t="s">
-        <v>33</v>
+      <c r="B13" s="143" t="s">
+        <v>32</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="11"/>
@@ -2786,9 +2790,9 @@
       </c>
     </row>
     <row r="14" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="149"/>
+      <c r="B14" s="148"/>
       <c r="C14" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="11"/>
@@ -2810,9 +2814,9 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="149"/>
+      <c r="B15" s="148"/>
       <c r="C15" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="11"/>
@@ -2834,9 +2838,9 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="149"/>
+      <c r="B16" s="148"/>
       <c r="C16" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="11"/>
@@ -2858,9 +2862,9 @@
       </c>
     </row>
     <row r="17" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="149"/>
+      <c r="B17" s="148"/>
       <c r="C17" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="11"/>
@@ -2870,7 +2874,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="41">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="J17" s="42" t="str">
         <f>IF(I17=100,"완료",IF(I17=0,"-","진행중"))</f>
@@ -2878,9 +2882,9 @@
       </c>
     </row>
     <row r="18" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="150"/>
+      <c r="B18" s="149"/>
       <c r="C18" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="11"/>
@@ -2909,7 +2913,7 @@
       <c r="H19" s="23"/>
       <c r="I19" s="17">
         <f>AVERAGE(I13:I18)</f>
-        <v>79.166666666666671</v>
+        <v>80.833333333333329</v>
       </c>
       <c r="J19" s="14">
         <f>COUNTIF(J13:J18,"완료")</f>
@@ -2917,11 +2921,11 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="144" t="s">
-        <v>38</v>
+      <c r="B20" s="143" t="s">
+        <v>37</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="11"/>
@@ -2943,9 +2947,9 @@
       </c>
     </row>
     <row r="21" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="149"/>
+      <c r="B21" s="148"/>
       <c r="C21" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="11"/>
@@ -2967,9 +2971,9 @@
       </c>
     </row>
     <row r="22" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="149"/>
+      <c r="B22" s="148"/>
       <c r="C22" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="11"/>
@@ -2991,9 +2995,9 @@
       </c>
     </row>
     <row r="23" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="149"/>
+      <c r="B23" s="148"/>
       <c r="C23" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="11"/>
@@ -3015,9 +3019,9 @@
       </c>
     </row>
     <row r="24" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="149"/>
+      <c r="B24" s="148"/>
       <c r="C24" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="11"/>
@@ -3039,9 +3043,9 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="149"/>
+      <c r="B25" s="148"/>
       <c r="C25" s="27" t="s">
-        <v>18</v>
+        <v>111</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="13"/>
@@ -3053,17 +3057,17 @@
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="47">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J25" s="48" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>진행중</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="150"/>
+      <c r="B26" s="149"/>
       <c r="C26" s="27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="13"/>
@@ -3075,7 +3079,7 @@
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="47">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="J26" s="61" t="str">
         <f t="shared" ref="J26" si="3">IF(I26=100,"완료",IF(I26=0,"-","진행중"))</f>
@@ -3092,7 +3096,7 @@
       <c r="H27" s="88"/>
       <c r="I27" s="89">
         <f>AVERAGE(I20:I26)</f>
-        <v>75</v>
+        <v>82.142857142857139</v>
       </c>
       <c r="J27" s="90">
         <f>COUNTIF(J20:J26,"완료")</f>
@@ -3100,11 +3104,11 @@
       </c>
     </row>
     <row r="28" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="144" t="s">
+      <c r="B28" s="143" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="98" t="s">
         <v>98</v>
-      </c>
-      <c r="C28" s="98" t="s">
-        <v>99</v>
       </c>
       <c r="D28" s="99"/>
       <c r="E28" s="100"/>
@@ -3117,18 +3121,18 @@
       <c r="H28" s="102">
         <v>44508</v>
       </c>
-      <c r="I28" s="106">
-        <v>1</v>
+      <c r="I28" s="159">
+        <v>100</v>
       </c>
       <c r="J28" s="105" t="str">
         <f>IF(I28=100,"완료",IF(I28=0,"-","진행중"))</f>
-        <v>진행중</v>
+        <v>완료</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="145"/>
+      <c r="B29" s="144"/>
       <c r="C29" s="98" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D29" s="99"/>
       <c r="E29" s="103"/>
@@ -3138,19 +3142,21 @@
       <c r="G29" s="101">
         <v>44517</v>
       </c>
-      <c r="H29" s="102"/>
-      <c r="I29" s="106">
-        <v>0</v>
+      <c r="H29" s="102">
+        <v>44508</v>
+      </c>
+      <c r="I29" s="159">
+        <v>100</v>
       </c>
       <c r="J29" s="105" t="str">
         <f>IF(I29=100,"완료",IF(I29=0,"-","진행중"))</f>
-        <v>-</v>
+        <v>완료</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="145"/>
+      <c r="B30" s="144"/>
       <c r="C30" s="98" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D30" s="99"/>
       <c r="E30" s="103"/>
@@ -3160,29 +3166,39 @@
       <c r="G30" s="101">
         <v>44517</v>
       </c>
-      <c r="H30" s="102"/>
-      <c r="I30" s="106">
-        <v>0</v>
+      <c r="H30" s="102">
+        <v>44515</v>
+      </c>
+      <c r="I30" s="159">
+        <v>100</v>
       </c>
       <c r="J30" s="105" t="str">
         <f>IF(I30=100,"완료",IF(I30=0,"-","진행중"))</f>
-        <v>-</v>
+        <v>완료</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="146"/>
-      <c r="C31" s="98"/>
+      <c r="B31" s="145"/>
+      <c r="C31" s="98" t="s">
+        <v>110</v>
+      </c>
       <c r="D31" s="99"/>
       <c r="E31" s="104"/>
-      <c r="F31" s="101"/>
-      <c r="G31" s="101"/>
-      <c r="H31" s="102"/>
-      <c r="I31" s="106">
-        <v>0</v>
+      <c r="F31" s="101">
+        <v>44478</v>
+      </c>
+      <c r="G31" s="101">
+        <v>44517</v>
+      </c>
+      <c r="H31" s="102">
+        <v>44508</v>
+      </c>
+      <c r="I31" s="159">
+        <v>100</v>
       </c>
       <c r="J31" s="105" t="str">
         <f>IF(I31=100,"완료",IF(I31=0,"-","진행중"))</f>
-        <v>-</v>
+        <v>완료</v>
       </c>
     </row>
     <row r="32" spans="2:10" s="16" customFormat="1" ht="11.25" x14ac:dyDescent="0.3">
@@ -3195,19 +3211,19 @@
       <c r="H32" s="95"/>
       <c r="I32" s="96">
         <f>AVERAGE(I28:I31)</f>
-        <v>0.25</v>
+        <v>100</v>
       </c>
       <c r="J32" s="97">
         <f>COUNTIF(J28:J31,"완료")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="144" t="s">
+      <c r="B33" s="143" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>42</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="11"/>
@@ -3227,9 +3243,9 @@
       </c>
     </row>
     <row r="34" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="149"/>
+      <c r="B34" s="148"/>
       <c r="C34" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="11"/>
@@ -3249,7 +3265,7 @@
       </c>
     </row>
     <row r="35" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="149"/>
+      <c r="B35" s="148"/>
       <c r="C35" s="27"/>
       <c r="D35" s="9"/>
       <c r="E35" s="13"/>
@@ -3265,7 +3281,7 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="150"/>
+      <c r="B36" s="149"/>
       <c r="C36" s="27"/>
       <c r="D36" s="9"/>
       <c r="E36" s="13"/>
@@ -3298,14 +3314,14 @@
       </c>
     </row>
     <row r="38" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="155" t="s">
+      <c r="B38" s="154" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D38" s="39"/>
-      <c r="E38" s="107"/>
+      <c r="E38" s="106"/>
       <c r="F38" s="7">
         <v>44481</v>
       </c>
@@ -3322,12 +3338,12 @@
       </c>
     </row>
     <row r="39" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="155"/>
+      <c r="B39" s="154"/>
       <c r="C39" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D39" s="39"/>
-      <c r="E39" s="107"/>
+      <c r="E39" s="106"/>
       <c r="F39" s="7">
         <v>44459</v>
       </c>
@@ -3344,12 +3360,12 @@
       </c>
     </row>
     <row r="40" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="155"/>
+      <c r="B40" s="154"/>
       <c r="C40" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D40" s="39"/>
-      <c r="E40" s="107"/>
+      <c r="E40" s="106"/>
       <c r="F40" s="7">
         <v>44459</v>
       </c>
@@ -3366,12 +3382,12 @@
       </c>
     </row>
     <row r="41" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="155"/>
+      <c r="B41" s="154"/>
       <c r="C41" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D41" s="39"/>
-      <c r="E41" s="107"/>
+      <c r="E41" s="106"/>
       <c r="F41" s="7">
         <v>44459</v>
       </c>
@@ -3388,12 +3404,12 @@
       </c>
     </row>
     <row r="42" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="155"/>
+      <c r="B42" s="154"/>
       <c r="C42" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D42" s="39"/>
-      <c r="E42" s="107"/>
+      <c r="E42" s="106"/>
       <c r="F42" s="7">
         <v>44459</v>
       </c>
@@ -3404,18 +3420,18 @@
       <c r="I42" s="41">
         <v>60</v>
       </c>
-      <c r="J42" s="108" t="str">
+      <c r="J42" s="107" t="str">
         <f>IF(I42=100,"완료",IF(I42=0,"-","진행중"))</f>
         <v>진행중</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="155"/>
+      <c r="B43" s="154"/>
       <c r="C43" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D43" s="39"/>
-      <c r="E43" s="107"/>
+      <c r="E43" s="106"/>
       <c r="F43" s="7">
         <v>44513</v>
       </c>
@@ -3426,18 +3442,18 @@
       <c r="I43" s="41">
         <v>0</v>
       </c>
-      <c r="J43" s="108" t="str">
+      <c r="J43" s="107" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="155"/>
+      <c r="B44" s="154"/>
       <c r="C44" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D44" s="39"/>
-      <c r="E44" s="107"/>
+      <c r="E44" s="106"/>
       <c r="F44" s="7">
         <v>44490</v>
       </c>
@@ -3448,7 +3464,7 @@
       <c r="I44" s="41">
         <v>50</v>
       </c>
-      <c r="J44" s="108" t="str">
+      <c r="J44" s="107" t="str">
         <f>IF(I44=100,"완료",IF(I44=0,"-","진행중"))</f>
         <v>진행중</v>
       </c>
@@ -3471,11 +3487,11 @@
       </c>
     </row>
     <row r="46" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="144" t="s">
+      <c r="B46" s="143" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="11"/>
@@ -3495,9 +3511,9 @@
       </c>
     </row>
     <row r="47" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="149"/>
+      <c r="B47" s="148"/>
       <c r="C47" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D47" s="39"/>
       <c r="E47" s="11"/>
@@ -3514,7 +3530,7 @@
       <c r="J47" s="4"/>
     </row>
     <row r="48" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="149"/>
+      <c r="B48" s="148"/>
       <c r="C48" s="5"/>
       <c r="D48" s="9"/>
       <c r="E48" s="11"/>
@@ -3525,7 +3541,7 @@
       <c r="J48" s="4"/>
     </row>
     <row r="49" spans="2:10" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="150"/>
+      <c r="B49" s="149"/>
       <c r="C49" s="5"/>
       <c r="D49" s="39"/>
       <c r="E49" s="11"/>
@@ -3556,7 +3572,7 @@
       </c>
     </row>
     <row r="51" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="144" t="s">
+      <c r="B51" s="143" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="5" t="s">
@@ -3580,7 +3596,7 @@
       </c>
     </row>
     <row r="52" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="149"/>
+      <c r="B52" s="148"/>
       <c r="C52" s="5" t="s">
         <v>9</v>
       </c>
@@ -3602,9 +3618,9 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="149"/>
+      <c r="B53" s="148"/>
       <c r="C53" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="11"/>
@@ -3624,7 +3640,7 @@
       </c>
     </row>
     <row r="54" spans="2:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="150"/>
+      <c r="B54" s="149"/>
       <c r="C54" s="5" t="s">
         <v>10</v>
       </c>
@@ -3776,98 +3792,98 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="71" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B1" s="71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="71" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="71" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I2" s="71" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="156" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="157" t="s">
+      <c r="A3" s="155" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="156" t="s">
+      <c r="B3" s="156" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="156" t="s">
+      <c r="C3" s="155" t="s">
         <v>80</v>
       </c>
-      <c r="E3" s="156" t="s">
+      <c r="D3" s="155" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="156" t="s">
+      <c r="E3" s="155" t="s">
         <v>78</v>
       </c>
-      <c r="G3" s="156" t="s">
+      <c r="F3" s="155" t="s">
         <v>77</v>
       </c>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156" t="s">
+      <c r="G3" s="155" t="s">
         <v>76</v>
       </c>
-      <c r="L3" s="156" t="s">
+      <c r="H3" s="155"/>
+      <c r="I3" s="155"/>
+      <c r="J3" s="155"/>
+      <c r="K3" s="155" t="s">
         <v>75</v>
       </c>
+      <c r="L3" s="155" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="4" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="156"/>
-      <c r="B4" s="158"/>
-      <c r="C4" s="156"/>
-      <c r="D4" s="156"/>
-      <c r="E4" s="156"/>
-      <c r="F4" s="156"/>
-      <c r="G4" s="156" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="156" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" s="156" t="s">
+      <c r="A4" s="155"/>
+      <c r="B4" s="157"/>
+      <c r="C4" s="155"/>
+      <c r="D4" s="155"/>
+      <c r="E4" s="155"/>
+      <c r="F4" s="155"/>
+      <c r="G4" s="155" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="155" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="156" t="s">
+      <c r="I4" s="155" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="155" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="156"/>
-      <c r="L4" s="156"/>
+      <c r="K4" s="155"/>
+      <c r="L4" s="155"/>
     </row>
     <row r="5" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="156"/>
-      <c r="B5" s="159"/>
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-      <c r="E5" s="156"/>
-      <c r="F5" s="156"/>
-      <c r="G5" s="156"/>
-      <c r="H5" s="156"/>
-      <c r="I5" s="156"/>
-      <c r="J5" s="156"/>
-      <c r="K5" s="156"/>
-      <c r="L5" s="156"/>
+      <c r="A5" s="155"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="155"/>
+      <c r="D5" s="155"/>
+      <c r="E5" s="155"/>
+      <c r="F5" s="155"/>
+      <c r="G5" s="155"/>
+      <c r="H5" s="155"/>
+      <c r="I5" s="155"/>
+      <c r="J5" s="155"/>
+      <c r="K5" s="155"/>
+      <c r="L5" s="155"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="79" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="79"/>
       <c r="C6" s="79" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D6" s="79"/>
       <c r="E6" s="79"/>
@@ -3883,10 +3899,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="75" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" s="75" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="75"/>
       <c r="D7" s="75"/>
@@ -4399,10 +4415,10 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="75" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="75" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C39" s="75"/>
       <c r="D39" s="75"/>
@@ -4499,10 +4515,10 @@
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="75" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45" s="75" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C45" s="75"/>
       <c r="D45" s="75"/>
@@ -4599,10 +4615,10 @@
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="75" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B51" s="75" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C51" s="75"/>
       <c r="D51" s="75"/>
@@ -4699,6 +4715,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="D3:D5"/>
     <mergeCell ref="L3:L5"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="G4:G5"/>
@@ -4706,12 +4728,6 @@
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K3:K5"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="D3:D5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4733,50 +4749,50 @@
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="157" t="s">
-        <v>82</v>
-      </c>
-      <c r="B1" s="156" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="156" t="s">
+      <c r="A1" s="156" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="155" t="s">
         <v>93</v>
       </c>
-      <c r="D1" s="157" t="s">
+      <c r="C1" s="155" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="157" t="s">
+      <c r="D1" s="156" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="157" t="s">
+      <c r="E1" s="156" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="157" t="s">
+      <c r="F1" s="156" t="s">
         <v>89</v>
       </c>
-      <c r="H1" s="157" t="s">
+      <c r="G1" s="156" t="s">
         <v>88</v>
       </c>
+      <c r="H1" s="156" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="158"/>
-      <c r="B2" s="156"/>
-      <c r="C2" s="156"/>
-      <c r="D2" s="158"/>
-      <c r="E2" s="158"/>
-      <c r="F2" s="158"/>
-      <c r="G2" s="158"/>
-      <c r="H2" s="158"/>
+      <c r="A2" s="157"/>
+      <c r="B2" s="155"/>
+      <c r="C2" s="155"/>
+      <c r="D2" s="157"/>
+      <c r="E2" s="157"/>
+      <c r="F2" s="157"/>
+      <c r="G2" s="157"/>
+      <c r="H2" s="157"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="158"/>
-      <c r="B3" s="157"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="158"/>
-      <c r="E3" s="159"/>
-      <c r="F3" s="159"/>
-      <c r="G3" s="158"/>
-      <c r="H3" s="158"/>
+      <c r="A3" s="157"/>
+      <c r="B3" s="156"/>
+      <c r="C3" s="156"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="158"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4806,10 +4822,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doc : WBS 업데이트
</commit_message>
<xml_diff>
--- a/Docs/WBS/WBS_Team_BlueBird.xlsx
+++ b/Docs/WBS/WBS_Team_BlueBird.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zereo\Desktop\Project\ContentsIT_Capston_Design\Docs\WBS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hhj32\Desktop\Contests_Capston\Git_ContentsIT_Capston_Design\Docs\WBS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BB2706-11D7-4630-B1B9-ADD0997B1C9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BE168E-9239-4E7E-AEFF-AC3F66A735BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3660" yWindow="5535" windowWidth="21600" windowHeight="11280" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MILESTONE" sheetId="2" r:id="rId1"/>
@@ -31,9 +31,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -1655,6 +1653,18 @@
     <xf numFmtId="178" fontId="13" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1746,18 +1756,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2180,72 +2178,72 @@
   <sheetData>
     <row r="1" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:21" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="117" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="113" t="s">
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="119"/>
+      <c r="F2" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="114"/>
-      <c r="H2" s="114"/>
-      <c r="I2" s="114"/>
-      <c r="J2" s="114"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="114"/>
-      <c r="M2" s="114"/>
-      <c r="N2" s="114"/>
-      <c r="O2" s="114"/>
-      <c r="P2" s="114"/>
-      <c r="Q2" s="114"/>
-      <c r="R2" s="114"/>
-      <c r="S2" s="114"/>
-      <c r="T2" s="114"/>
-      <c r="U2" s="115"/>
+      <c r="G2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="118"/>
+      <c r="M2" s="118"/>
+      <c r="N2" s="118"/>
+      <c r="O2" s="118"/>
+      <c r="P2" s="118"/>
+      <c r="Q2" s="118"/>
+      <c r="R2" s="118"/>
+      <c r="S2" s="118"/>
+      <c r="T2" s="118"/>
+      <c r="U2" s="119"/>
     </row>
     <row r="3" spans="2:21" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="134" t="s">
+      <c r="B3" s="138" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="120" t="s">
+      <c r="C3" s="124" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="130" t="s">
+      <c r="D3" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="131"/>
-      <c r="F3" s="125" t="s">
+      <c r="E3" s="135"/>
+      <c r="F3" s="129" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="126"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="122" t="s">
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="131"/>
+      <c r="J3" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="124"/>
-      <c r="N3" s="125" t="s">
+      <c r="K3" s="127"/>
+      <c r="L3" s="127"/>
+      <c r="M3" s="128"/>
+      <c r="N3" s="129" t="s">
         <v>30</v>
       </c>
-      <c r="O3" s="126"/>
-      <c r="P3" s="126"/>
-      <c r="Q3" s="127"/>
-      <c r="R3" s="122" t="s">
+      <c r="O3" s="130"/>
+      <c r="P3" s="130"/>
+      <c r="Q3" s="131"/>
+      <c r="R3" s="126" t="s">
         <v>57</v>
       </c>
-      <c r="S3" s="123"/>
-      <c r="T3" s="123"/>
-      <c r="U3" s="124"/>
+      <c r="S3" s="127"/>
+      <c r="T3" s="127"/>
+      <c r="U3" s="128"/>
     </row>
     <row r="4" spans="2:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="135"/>
-      <c r="C4" s="121"/>
-      <c r="D4" s="132"/>
-      <c r="E4" s="133"/>
+      <c r="B4" s="139"/>
+      <c r="C4" s="125"/>
+      <c r="D4" s="136"/>
+      <c r="E4" s="137"/>
       <c r="F4" s="54" t="s">
         <v>12</v>
       </c>
@@ -2296,16 +2294,16 @@
       </c>
     </row>
     <row r="5" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="116">
+      <c r="B5" s="120">
         <v>1</v>
       </c>
       <c r="C5" s="43">
         <v>44440</v>
       </c>
-      <c r="D5" s="136" t="s">
+      <c r="D5" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="137"/>
+      <c r="E5" s="141"/>
       <c r="F5" s="35"/>
       <c r="G5" s="51"/>
       <c r="H5" s="52"/>
@@ -2324,14 +2322,14 @@
       <c r="U5" s="34"/>
     </row>
     <row r="6" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="117"/>
-      <c r="C6" s="119" t="s">
+      <c r="B6" s="121"/>
+      <c r="C6" s="123" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="138" t="s">
+      <c r="D6" s="142" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="139"/>
+      <c r="E6" s="143"/>
       <c r="F6" s="38"/>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
@@ -2350,12 +2348,12 @@
       <c r="U6" s="34"/>
     </row>
     <row r="7" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="117"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="140" t="s">
+      <c r="B7" s="121"/>
+      <c r="C7" s="123"/>
+      <c r="D7" s="109" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="141"/>
+      <c r="E7" s="110"/>
       <c r="F7" s="33"/>
       <c r="G7" s="32"/>
       <c r="H7" s="32"/>
@@ -2374,12 +2372,12 @@
       <c r="U7" s="34"/>
     </row>
     <row r="8" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="117"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="142" t="s">
+      <c r="B8" s="121"/>
+      <c r="C8" s="123"/>
+      <c r="D8" s="111" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="143"/>
+      <c r="E8" s="112"/>
       <c r="F8" s="33"/>
       <c r="G8" s="32"/>
       <c r="H8" s="32"/>
@@ -2397,12 +2395,12 @@
       <c r="U8" s="34"/>
     </row>
     <row r="9" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="117"/>
-      <c r="C9" s="119"/>
-      <c r="D9" s="109" t="s">
+      <c r="B9" s="121"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="110"/>
+      <c r="E9" s="114"/>
       <c r="F9" s="35"/>
       <c r="G9" s="31"/>
       <c r="H9" s="32"/>
@@ -2421,12 +2419,12 @@
       <c r="U9" s="34"/>
     </row>
     <row r="10" spans="2:21" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="117"/>
-      <c r="C10" s="119"/>
-      <c r="D10" s="111" t="s">
+      <c r="B10" s="121"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="112"/>
+      <c r="E10" s="116"/>
       <c r="F10" s="35"/>
       <c r="G10" s="31"/>
       <c r="H10" s="32"/>
@@ -2445,14 +2443,14 @@
       <c r="U10" s="34"/>
     </row>
     <row r="11" spans="2:21" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="118"/>
+      <c r="B11" s="122"/>
       <c r="C11" s="44">
         <v>44532</v>
       </c>
-      <c r="D11" s="128" t="s">
+      <c r="D11" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="129"/>
+      <c r="E11" s="133"/>
       <c r="F11" s="36"/>
       <c r="G11" s="37"/>
       <c r="H11" s="62"/>
@@ -2472,6 +2470,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
@@ -2488,8 +2488,6 @@
     <mergeCell ref="N3:Q3"/>
     <mergeCell ref="R3:U3"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2509,8 +2507,8 @@
   </sheetPr>
   <dimension ref="B1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2598,7 +2596,7 @@
       </c>
       <c r="I5" s="3">
         <f>AVERAGE(I12,I19,I27,I45,I50,I55,I37)</f>
-        <v>44.183673469387756</v>
+        <v>45.612244897959179</v>
       </c>
       <c r="J5" s="2">
         <f>COUNTIF(J6:J55,"완료")</f>
@@ -3330,7 +3328,7 @@
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="41">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="J38" s="42" t="str">
         <f t="shared" ref="J38:J43" si="5">IF(I38=100,"완료",IF(I38=0,"-","진행중"))</f>
@@ -3352,7 +3350,7 @@
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="41">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="J39" s="42" t="str">
         <f t="shared" si="5"/>
@@ -3374,7 +3372,7 @@
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="41">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="J40" s="42" t="str">
         <f t="shared" si="5"/>
@@ -3396,7 +3394,7 @@
       </c>
       <c r="H41" s="7"/>
       <c r="I41" s="41">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="J41" s="42" t="str">
         <f t="shared" si="5"/>
@@ -3418,7 +3416,7 @@
       </c>
       <c r="H42" s="40"/>
       <c r="I42" s="41">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="J42" s="107" t="str">
         <f>IF(I42=100,"완료",IF(I42=0,"-","진행중"))</f>
@@ -3462,7 +3460,7 @@
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="41">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="J44" s="107" t="str">
         <f>IF(I44=100,"완료",IF(I44=0,"-","진행중"))</f>
@@ -3479,7 +3477,7 @@
       <c r="H45" s="23"/>
       <c r="I45" s="17">
         <f>AVERAGE(I38:I44)</f>
-        <v>46.428571428571431</v>
+        <v>56.428571428571431</v>
       </c>
       <c r="J45" s="14">
         <f>COUNTIF(J38:J44,"완료")</f>
@@ -4715,6 +4713,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="F3:F5"/>
+    <mergeCell ref="D3:D5"/>
     <mergeCell ref="L3:L5"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="G4:G5"/>
@@ -4722,12 +4726,6 @@
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K3:K5"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="D3:D5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>